<commit_message>
Add wandb, change cnn
</commit_message>
<xml_diff>
--- a/Logs/debug/testing_episode_output.xlsx
+++ b/Logs/debug/testing_episode_output.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,58 +405,58 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B2">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1.120000004768372</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>5.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.3899999856948853</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1.389999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-1</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B4">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C4">
-        <v>0.7300000190734863</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D4">
-        <v>3.703703641891479</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-1.669999957084656</v>
+        <v>-1</v>
       </c>
       <c r="B5">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1.399999976158142</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>6.185184955596924</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -489,16 +489,16 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>-1.590000033378601</v>
+        <v>-1</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.5900000333786011</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1.590000033378601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -520,35 +520,35 @@
         <v>-1</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>-1.730000019073486</v>
+        <v>-1.100000023841858</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C11">
-        <v>0.7300000190734863</v>
+        <v>0.7100000381469727</v>
       </c>
       <c r="D11">
-        <v>1.730000019073486</v>
+        <v>2.820513010025024</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B12">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -562,13 +562,13 @@
         <v>-1</v>
       </c>
       <c r="B13">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C13">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D13">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -587,16 +587,16 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>-1.669999957084656</v>
+        <v>-2.529999971389771</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C15">
-        <v>0.6699999570846558</v>
+        <v>2.139999866485596</v>
       </c>
       <c r="D15">
-        <v>1.669999957084656</v>
+        <v>6.487179756164551</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -604,55 +604,55 @@
         <v>-1</v>
       </c>
       <c r="B16">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>-1.460000038146973</v>
+        <v>-1</v>
       </c>
       <c r="B17">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>1.190000057220459</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>5.407407283782959</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>-1.879999995231628</v>
+        <v>-1.389999985694885</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C18">
-        <v>0.8799999952316284</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>1.879999995231628</v>
+        <v>3.564102649688721</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>-1.139999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B19">
-        <v>0.2700000107288361</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C19">
-        <v>0.8700000047683716</v>
+        <v>0.6899999976158142</v>
       </c>
       <c r="D19">
-        <v>4.222221851348877</v>
+        <v>3.225806474685669</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -660,13 +660,13 @@
         <v>-1</v>
       </c>
       <c r="B20">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -674,35 +674,35 @@
         <v>-1</v>
       </c>
       <c r="B21">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C21">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D21">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>-1.570000052452087</v>
+        <v>-1</v>
       </c>
       <c r="B22">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>1.300000071525574</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>5.814814567565918</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B23">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>-1.379999995231628</v>
+        <v>-1.039999961853027</v>
       </c>
       <c r="B25">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C25">
-        <v>1.110000014305115</v>
+        <v>0.6499999761581421</v>
       </c>
       <c r="D25">
-        <v>5.111110687255859</v>
+        <v>2.666666746139526</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -755,44 +755,44 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>-1</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B28">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C28">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>-1.590000033378601</v>
+        <v>-1</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0.5900000333786011</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1.590000033378601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -800,27 +800,27 @@
         <v>-1</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>-1</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>3.307692289352417</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -828,77 +828,77 @@
         <v>-1</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.6899999976158142</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>3.225806474685669</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>-1</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>3.307692289352417</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>-1.710000038146973</v>
+        <v>-0.9399999976158142</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C34">
-        <v>0.7100000381469727</v>
+        <v>0.550000011920929</v>
       </c>
       <c r="D34">
-        <v>1.710000038146973</v>
+        <v>2.410256385803223</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>-1.669999957084656</v>
+        <v>-1</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35">
-        <v>0.6699999570846558</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>1.669999957084656</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>-1.529999971389771</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B36">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C36">
-        <v>1.259999990463257</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D36">
-        <v>5.666666507720947</v>
+        <v>3.307692289352417</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>-0.2700000107288361</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B37">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -926,13 +926,13 @@
         <v>-1</v>
       </c>
       <c r="B39">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -940,13 +940,13 @@
         <v>-1</v>
       </c>
       <c r="B40">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C40">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D40">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -954,13 +954,13 @@
         <v>-1</v>
       </c>
       <c r="B41">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C41">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D41">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -968,27 +968,27 @@
         <v>-1</v>
       </c>
       <c r="B42">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C42">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D42">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>-1</v>
+        <v>-0.4900000095367432</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.1000000238418579</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>1.256410360336304</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -996,13 +996,13 @@
         <v>-1</v>
       </c>
       <c r="B44">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1010,41 +1010,41 @@
         <v>-1</v>
       </c>
       <c r="B45">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>-1.590000033378601</v>
+        <v>-1</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46">
-        <v>0.5900000333786011</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>1.590000033378601</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>-1</v>
+        <v>-0.800000011920929</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>0.4100000262260437</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>2.051282167434692</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1052,21 +1052,21 @@
         <v>-1</v>
       </c>
       <c r="B48">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C48">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D48">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1077,44 +1077,44 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>-1</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1.550000071525574</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>4.974359512329102</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>-1.710000038146973</v>
+        <v>-1</v>
       </c>
       <c r="B51">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>1.440000057220459</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>6.333333015441895</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
-        <v>-1</v>
+        <v>-0.6899999976158142</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.300000011920929</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>1.769230842590332</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1133,38 +1133,38 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B54">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
-        <v>-1.389999985694885</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C55">
-        <v>0.3899999856948853</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>1.389999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B56">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1175,24 +1175,24 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>-1.549999952316284</v>
+        <v>-1</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>0.5499999523162842</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>1.549999952316284</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B58">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1203,44 +1203,44 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>-1.570000052452087</v>
+        <v>-1</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C59">
-        <v>0.5700000524520874</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D59">
-        <v>1.570000052452087</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>-0.3499999940395355</v>
+        <v>-0.7400000095367432</v>
       </c>
       <c r="B60">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C60">
-        <v>0.07999998331069946</v>
+        <v>0.3500000238418579</v>
       </c>
       <c r="D60">
-        <v>1.296296238899231</v>
+        <v>1.897436022758484</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>-1</v>
+        <v>-0.949999988079071</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.6399999856948853</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>3.064516067504883</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1248,13 +1248,13 @@
         <v>-1</v>
       </c>
       <c r="B62">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C62">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D62">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1273,86 +1273,86 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
-        <v>-1.659999966621399</v>
+        <v>-1</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C64">
-        <v>0.6599999666213989</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D64">
-        <v>1.659999966621399</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>-0.5799999833106995</v>
+        <v>-1</v>
       </c>
       <c r="B65">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>0.3099999725818634</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>2.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B66">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>1.120000004768372</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>5.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>-1.139999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67">
-        <v>0.1399999856948853</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>1.139999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68">
-        <v>-0.6299999952316284</v>
+        <v>-1</v>
       </c>
       <c r="B68">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>0.3599999845027924</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>2.333333253860474</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>-1.840000033378601</v>
+        <v>-1</v>
       </c>
       <c r="B69">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>1.570000052452087</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>6.814814567565918</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1371,30 +1371,30 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71">
-        <v>-1.720000028610229</v>
+        <v>-1</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71">
-        <v>0.7200000286102295</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>1.720000028610229</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72">
-        <v>-1</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1402,13 +1402,13 @@
         <v>-1</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1430,27 +1430,27 @@
         <v>-1</v>
       </c>
       <c r="B75">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C75">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D75">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76">
-        <v>-1.659999966621399</v>
+        <v>-1</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76">
-        <v>0.6599999666213989</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>1.659999966621399</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1458,35 +1458,35 @@
         <v>-1</v>
       </c>
       <c r="B77">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C77">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D77">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78">
-        <v>-1</v>
+        <v>-0.8899999856948853</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>2.28205132484436</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B79">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1497,52 +1497,52 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B80">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>1.120000004768372</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>5.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81">
-        <v>-1.590000033378601</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B81">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C81">
-        <v>1.320000052452087</v>
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>5.888888835906982</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82">
-        <v>-1.639999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82">
-        <v>0.6399999856948853</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>1.639999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1553,16 +1553,16 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84">
-        <v>-1.590000033378601</v>
+        <v>-1</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C84">
-        <v>0.5900000333786011</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D84">
-        <v>1.590000033378601</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1581,58 +1581,58 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B86">
         <v>1</v>
       </c>
       <c r="C86">
-        <v>0.3899999856948853</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>1.389999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87">
-        <v>-1.590000033378601</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C87">
-        <v>0.5900000333786011</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D87">
-        <v>1.590000033378601</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88">
-        <v>-1.960000038146973</v>
+        <v>-1</v>
       </c>
       <c r="B88">
         <v>1</v>
       </c>
       <c r="C88">
-        <v>0.9600000381469727</v>
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>1.960000038146973</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89">
-        <v>-1</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B89">
-        <v>0.2700000107288361</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C89">
-        <v>0.7300000190734863</v>
+        <v>0.9799999594688416</v>
       </c>
       <c r="D89">
-        <v>3.703703641891479</v>
+        <v>4.161290168762207</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1640,63 +1640,63 @@
         <v>-1</v>
       </c>
       <c r="B90">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C90">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91">
-        <v>-1.730000019073486</v>
+        <v>-1</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>1.730000019073486</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92">
-        <v>-1.850000023841858</v>
+        <v>-1</v>
       </c>
       <c r="B92">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C92">
-        <v>1.580000042915344</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D92">
-        <v>6.851851463317871</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93">
-        <v>-0.9300000071525574</v>
+        <v>-1</v>
       </c>
       <c r="B93">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C93">
-        <v>0.6599999666213989</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>3.444444417953491</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95">
-        <v>-0.2700000107288361</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B95">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1724,35 +1724,35 @@
         <v>-1</v>
       </c>
       <c r="B96">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C96">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D96">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97">
-        <v>-1</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B97">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C97">
-        <v>0.7300000190734863</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D97">
-        <v>3.703703641891479</v>
+        <v>3.307692289352417</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -1794,13 +1794,13 @@
         <v>-1</v>
       </c>
       <c r="B101">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C101">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D101">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1808,49 +1808,49 @@
         <v>-1</v>
       </c>
       <c r="B102">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C102">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B103">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104">
-        <v>-1.710000038146973</v>
+        <v>-1</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104">
-        <v>0.7100000381469727</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>1.710000038146973</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B105">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -1864,13 +1864,13 @@
         <v>-1</v>
       </c>
       <c r="B106">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1878,21 +1878,21 @@
         <v>-1</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.6899999976158142</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>3.225806474685669</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B108">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -1903,16 +1903,16 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109">
-        <v>-1.389999985694885</v>
+        <v>-0.8299999833106995</v>
       </c>
       <c r="B109">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C109">
-        <v>1.120000004768372</v>
+        <v>0.4399999976158142</v>
       </c>
       <c r="D109">
-        <v>5.148148059844971</v>
+        <v>2.128205060958862</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1931,30 +1931,30 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111">
-        <v>-1.659999966621399</v>
+        <v>-1</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111">
-        <v>0.6599999666213989</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>1.659999966621399</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112">
-        <v>-1.960000038146973</v>
+        <v>-0.6299999952316284</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C112">
-        <v>0.9600000381469727</v>
+        <v>0.2400000095367432</v>
       </c>
       <c r="D112">
-        <v>1.960000038146973</v>
+        <v>1.615384697914124</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1962,27 +1962,27 @@
         <v>-1</v>
       </c>
       <c r="B113">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C113">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D113">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114">
-        <v>-0.3499999940395355</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B114">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C114">
-        <v>0.07999998331069946</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D114">
-        <v>1.296296238899231</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1990,13 +1990,13 @@
         <v>-1</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2018,13 +2018,13 @@
         <v>-1</v>
       </c>
       <c r="B117">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C117">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D117">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2032,13 +2032,13 @@
         <v>-1</v>
       </c>
       <c r="B118">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C118">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D118">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2046,91 +2046,91 @@
         <v>-1</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120">
-        <v>-1</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>0.2199999690055847</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>1.709677338600159</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121">
-        <v>-1.570000052452087</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C121">
-        <v>0.5700000524520874</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>1.570000052452087</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B122">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C122">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123">
-        <v>-1.659999966621399</v>
+        <v>-1</v>
       </c>
       <c r="B123">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C123">
-        <v>1.389999985694885</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>6.148147583007812</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124">
-        <v>-1</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B124">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C124">
-        <v>0.7300000190734863</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D124">
-        <v>3.703703641891479</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B125">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -2144,27 +2144,27 @@
         <v>-1.669999957084656</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C126">
-        <v>0.6699999570846558</v>
+        <v>1.279999971389771</v>
       </c>
       <c r="D126">
-        <v>1.669999957084656</v>
+        <v>4.282051563262939</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127">
-        <v>-0.2700000107288361</v>
+        <v>-1</v>
       </c>
       <c r="B127">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2172,41 +2172,41 @@
         <v>-1</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129">
-        <v>-1.669999957084656</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C129">
-        <v>0.6699999570846558</v>
+        <v>0</v>
       </c>
       <c r="D129">
-        <v>1.669999957084656</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130">
-        <v>-1.700000047683716</v>
+        <v>-1.850000023841858</v>
       </c>
       <c r="B130">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C130">
-        <v>1.430000066757202</v>
+        <v>1.460000038146973</v>
       </c>
       <c r="D130">
-        <v>6.296296119689941</v>
+        <v>4.743589878082275</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2214,27 +2214,27 @@
         <v>-1</v>
       </c>
       <c r="B131">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C131">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132">
-        <v>-1</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>3.307692289352417</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2253,30 +2253,30 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134">
-        <v>-1.570000052452087</v>
+        <v>-1</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C134">
-        <v>0.5700000524520874</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D134">
-        <v>1.570000052452087</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B135">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C135">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2284,13 +2284,13 @@
         <v>-1</v>
       </c>
       <c r="B136">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C136">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D136">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2298,27 +2298,27 @@
         <v>-1</v>
       </c>
       <c r="B137">
-        <v>0.2700000107288361</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C137">
-        <v>0.7300000190734863</v>
+        <v>0.6899999976158142</v>
       </c>
       <c r="D137">
-        <v>3.703703641891479</v>
+        <v>3.225806474685669</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138">
-        <v>-1.419999957084656</v>
+        <v>-1</v>
       </c>
       <c r="B138">
         <v>1</v>
       </c>
       <c r="C138">
-        <v>0.4199999570846558</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>1.419999957084656</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2337,58 +2337,58 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.07999998331069946</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>1.25806450843811</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141">
-        <v>-1</v>
+        <v>-1.200000047683716</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>0.89000004529953</v>
       </c>
       <c r="D141">
-        <v>1</v>
+        <v>3.870967864990234</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B142">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C142">
-        <v>1.120000004768372</v>
+        <v>0</v>
       </c>
       <c r="D142">
-        <v>5.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143">
-        <v>-0.2700000107288361</v>
+        <v>-0.449999988079071</v>
       </c>
       <c r="B143">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>0.06000000238418579</v>
       </c>
       <c r="D143">
-        <v>1</v>
+        <v>1.153846144676208</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2396,13 +2396,13 @@
         <v>-1</v>
       </c>
       <c r="B144">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C144">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2410,83 +2410,83 @@
         <v>-1</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D145">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146">
-        <v>-1.759999990463257</v>
+        <v>-1</v>
       </c>
       <c r="B146">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C146">
-        <v>1.490000009536743</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D146">
-        <v>6.518518447875977</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147">
-        <v>-1.879999995231628</v>
+        <v>-0.9800000190734863</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C147">
-        <v>0.8799999952316284</v>
+        <v>0.5900000333786011</v>
       </c>
       <c r="D147">
-        <v>1.879999995231628</v>
+        <v>2.512820720672607</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148">
-        <v>-1.419999957084656</v>
+        <v>-1</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
       <c r="C148">
-        <v>0.4199999570846558</v>
+        <v>0</v>
       </c>
       <c r="D148">
-        <v>1.419999957084656</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149">
-        <v>-1.659999966621399</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C149">
-        <v>0.6599999666213989</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D149">
-        <v>1.659999966621399</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150">
-        <v>-1.389999985694885</v>
+        <v>-0.8899999856948853</v>
       </c>
       <c r="B150">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C150">
-        <v>1.120000004768372</v>
+        <v>0.5</v>
       </c>
       <c r="D150">
-        <v>5.148148059844971</v>
+        <v>2.28205132484436</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2494,13 +2494,13 @@
         <v>-1</v>
       </c>
       <c r="B151">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C151">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D151">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2508,27 +2508,27 @@
         <v>-1</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153">
-        <v>-1</v>
+        <v>-0.5299999713897705</v>
       </c>
       <c r="B153">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C153">
-        <v>0.7300000190734863</v>
+        <v>0.1399999856948853</v>
       </c>
       <c r="D153">
-        <v>3.703703641891479</v>
+        <v>1.35897433757782</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2547,30 +2547,30 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155">
-        <v>-1</v>
+        <v>-0.4900000095367432</v>
       </c>
       <c r="B155">
-        <v>0.2700000107288361</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C155">
-        <v>0.7300000190734863</v>
+        <v>0.1800000071525574</v>
       </c>
       <c r="D155">
-        <v>3.703703641891479</v>
+        <v>1.580645203590393</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156">
-        <v>-0.6600000262260437</v>
+        <v>-0.75</v>
       </c>
       <c r="B156">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C156">
-        <v>0.3900000154972076</v>
+        <v>0.3600000143051147</v>
       </c>
       <c r="D156">
-        <v>2.444444417953491</v>
+        <v>1.923076987266541</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2592,13 +2592,13 @@
         <v>-1</v>
       </c>
       <c r="B158">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C158">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D158">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2606,55 +2606,55 @@
         <v>-1</v>
       </c>
       <c r="B159">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C159">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D159">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160">
-        <v>-1.139999985694885</v>
+        <v>-1.980000019073486</v>
       </c>
       <c r="B160">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C160">
-        <v>0.8700000047683716</v>
+        <v>1.590000033378601</v>
       </c>
       <c r="D160">
-        <v>4.222221851348877</v>
+        <v>5.076923370361328</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161">
-        <v>-1</v>
+        <v>-0.8399999737739563</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>0.449999988079071</v>
       </c>
       <c r="D161">
-        <v>1</v>
+        <v>2.153846263885498</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162">
-        <v>-1.139999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B162">
         <v>1</v>
       </c>
       <c r="C162">
-        <v>0.1399999856948853</v>
+        <v>0</v>
       </c>
       <c r="D162">
-        <v>1.139999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2662,55 +2662,55 @@
         <v>-1</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D163">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164">
-        <v>-1.740000009536743</v>
+        <v>-0.8899999856948853</v>
       </c>
       <c r="B164">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C164">
-        <v>0.7400000095367432</v>
+        <v>0.5</v>
       </c>
       <c r="D164">
-        <v>1.740000009536743</v>
+        <v>2.28205132484436</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165">
-        <v>-0.2700000107288361</v>
+        <v>-1.25</v>
       </c>
       <c r="B165">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>0.8600000143051147</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>3.20512843132019</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166">
-        <v>-1.659999966621399</v>
+        <v>-1</v>
       </c>
       <c r="B166">
         <v>1</v>
       </c>
       <c r="C166">
-        <v>0.6599999666213989</v>
+        <v>0</v>
       </c>
       <c r="D166">
-        <v>1.659999966621399</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2732,13 +2732,13 @@
         <v>-1</v>
       </c>
       <c r="B168">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C168">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D168">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2746,13 +2746,13 @@
         <v>-1</v>
       </c>
       <c r="B169">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C169">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D169">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2771,30 +2771,30 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171">
-        <v>-0.2700000107288361</v>
+        <v>-0.8700000047683716</v>
       </c>
       <c r="B171">
-        <v>0.2700000107288361</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C171">
-        <v>0</v>
+        <v>0.5600000023841858</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>2.806451559066772</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172">
-        <v>-1</v>
+        <v>-0.449999988079071</v>
       </c>
       <c r="B172">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C172">
-        <v>0.7300000190734863</v>
+        <v>0.06000000238418579</v>
       </c>
       <c r="D172">
-        <v>3.703703641891479</v>
+        <v>1.153846144676208</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2802,35 +2802,35 @@
         <v>-1</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D173">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174">
-        <v>-1.759999990463257</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C174">
-        <v>0.7599999904632568</v>
+        <v>0</v>
       </c>
       <c r="D174">
-        <v>1.759999990463257</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176">
-        <v>-1</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -2858,69 +2858,69 @@
         <v>-1</v>
       </c>
       <c r="B177">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C177">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D177">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B178">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C178">
-        <v>1.120000004768372</v>
+        <v>0</v>
       </c>
       <c r="D178">
-        <v>5.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179">
-        <v>-0.2700000107288361</v>
+        <v>-1.289999961853027</v>
       </c>
       <c r="B179">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C179">
-        <v>0</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D179">
-        <v>1</v>
+        <v>3.307692289352417</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180">
-        <v>-0.5799999833106995</v>
+        <v>-1</v>
       </c>
       <c r="B180">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C180">
-        <v>0.3099999725818634</v>
+        <v>0</v>
       </c>
       <c r="D180">
-        <v>2.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181">
-        <v>-1.590000033378601</v>
+        <v>-0.8399999737739563</v>
       </c>
       <c r="B181">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C181">
-        <v>1.320000052452087</v>
+        <v>0.449999988079071</v>
       </c>
       <c r="D181">
-        <v>5.888888835906982</v>
+        <v>2.153846263885498</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2942,13 +2942,13 @@
         <v>-1</v>
       </c>
       <c r="B183">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C183">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D183">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2967,16 +2967,16 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185">
-        <v>-1.659999966621399</v>
+        <v>-1</v>
       </c>
       <c r="B185">
         <v>1</v>
       </c>
       <c r="C185">
-        <v>0.6599999666213989</v>
+        <v>0</v>
       </c>
       <c r="D185">
-        <v>1.659999966621399</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -2984,13 +2984,13 @@
         <v>-1</v>
       </c>
       <c r="B186">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C186">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D186">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -2998,55 +2998,55 @@
         <v>-1</v>
       </c>
       <c r="B187">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C187">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D187">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188">
-        <v>-1.570000052452087</v>
+        <v>-1</v>
       </c>
       <c r="B188">
         <v>1</v>
       </c>
       <c r="C188">
-        <v>0.5700000524520874</v>
+        <v>0</v>
       </c>
       <c r="D188">
-        <v>1.570000052452087</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189">
-        <v>-0.4000000059604645</v>
+        <v>-1</v>
       </c>
       <c r="B189">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C189">
-        <v>0.1299999952316284</v>
+        <v>0</v>
       </c>
       <c r="D189">
-        <v>1.481481432914734</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190">
-        <v>-1.669999957084656</v>
+        <v>-1</v>
       </c>
       <c r="B190">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C190">
-        <v>1.399999976158142</v>
+        <v>0</v>
       </c>
       <c r="D190">
-        <v>6.185184955596924</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3054,13 +3054,13 @@
         <v>-1</v>
       </c>
       <c r="B191">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C191">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D191">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3079,44 +3079,44 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193">
-        <v>-1.389999985694885</v>
+        <v>-0.3899999856948853</v>
       </c>
       <c r="B193">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C193">
-        <v>1.120000004768372</v>
+        <v>0</v>
       </c>
       <c r="D193">
-        <v>5.148148059844971</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194">
-        <v>-1</v>
+        <v>-0.449999988079071</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C194">
-        <v>0</v>
+        <v>0.06000000238418579</v>
       </c>
       <c r="D194">
-        <v>1</v>
+        <v>1.153846144676208</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195">
-        <v>-1</v>
+        <v>-1.389999985694885</v>
       </c>
       <c r="B195">
-        <v>0.2700000107288361</v>
+        <v>0.3100000023841858</v>
       </c>
       <c r="C195">
-        <v>0.7300000190734863</v>
+        <v>1.079999923706055</v>
       </c>
       <c r="D195">
-        <v>3.703703641891479</v>
+        <v>4.483870983123779</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3124,13 +3124,13 @@
         <v>-1</v>
       </c>
       <c r="B196">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C196">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D196">
-        <v>3.703703641891479</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3138,55 +3138,55 @@
         <v>-1</v>
       </c>
       <c r="B197">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C197">
-        <v>0.7300000190734863</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D197">
-        <v>3.703703641891479</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="B198">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C198">
-        <v>0.7300000190734863</v>
+        <v>0.3600000143051147</v>
       </c>
       <c r="D198">
-        <v>3.703703641891479</v>
+        <v>1.923076987266541</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199">
-        <v>-1.139999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B199">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C199">
-        <v>0.8700000047683716</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D199">
-        <v>4.222221851348877</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200">
-        <v>-1</v>
+        <v>-1.100000023841858</v>
       </c>
       <c r="B200">
-        <v>0.2700000107288361</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C200">
-        <v>0.7300000190734863</v>
+        <v>0.7100000381469727</v>
       </c>
       <c r="D200">
-        <v>3.703703641891479</v>
+        <v>2.820513010025024</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3219,16 +3219,16 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203">
-        <v>-1.379999995231628</v>
+        <v>-1</v>
       </c>
       <c r="B203">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C203">
-        <v>1.110000014305115</v>
+        <v>0</v>
       </c>
       <c r="D203">
-        <v>5.111110687255859</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3250,13 +3250,13 @@
         <v>-1</v>
       </c>
       <c r="B205">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C205">
-        <v>0</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D205">
-        <v>1</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3275,30 +3275,30 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B207">
         <v>1</v>
       </c>
       <c r="C207">
-        <v>0.3899999856948853</v>
+        <v>0</v>
       </c>
       <c r="D207">
-        <v>1.389999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208">
-        <v>-1.600000023841858</v>
+        <v>-1</v>
       </c>
       <c r="B208">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C208">
-        <v>0.6000000238418579</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D208">
-        <v>1.600000023841858</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3317,30 +3317,30 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210">
-        <v>-1.710000038146973</v>
+        <v>-1</v>
       </c>
       <c r="B210">
-        <v>1</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="C210">
-        <v>0.7100000381469727</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="D210">
-        <v>1.710000038146973</v>
+        <v>2.564102649688721</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211">
-        <v>-1.389999985694885</v>
+        <v>-1</v>
       </c>
       <c r="B211">
         <v>1</v>
       </c>
       <c r="C211">
-        <v>0.3899999856948853</v>
+        <v>0</v>
       </c>
       <c r="D211">
-        <v>1.389999985694885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3348,13 +3348,503 @@
         <v>-1</v>
       </c>
       <c r="B212">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C212">
-        <v>0.7300000190734863</v>
+        <v>0</v>
       </c>
       <c r="D212">
-        <v>3.703703641891479</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213">
+        <v>-1</v>
+      </c>
+      <c r="B213">
+        <v>1</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214">
+        <v>-1</v>
+      </c>
+      <c r="B214">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C214">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D214">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215">
+        <v>-1</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216">
+        <v>-1</v>
+      </c>
+      <c r="B216">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C216">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D216">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217">
+        <v>-1.389999985694885</v>
+      </c>
+      <c r="B217">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217">
+        <v>3.564102649688721</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218">
+        <v>-1</v>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219">
+        <v>-1</v>
+      </c>
+      <c r="B219">
+        <v>1</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220">
+        <v>-1</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+      <c r="D220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221">
+        <v>-1</v>
+      </c>
+      <c r="B221">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C221">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D221">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222">
+        <v>-1</v>
+      </c>
+      <c r="B222">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C222">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D222">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223">
+        <v>-1</v>
+      </c>
+      <c r="B223">
+        <v>1</v>
+      </c>
+      <c r="C223">
+        <v>0</v>
+      </c>
+      <c r="D223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224">
+        <v>-1</v>
+      </c>
+      <c r="B224">
+        <v>1</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225">
+        <v>-1</v>
+      </c>
+      <c r="B225">
+        <v>1</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226">
+        <v>-1</v>
+      </c>
+      <c r="B226">
+        <v>1</v>
+      </c>
+      <c r="C226">
+        <v>0</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227">
+        <v>-1</v>
+      </c>
+      <c r="B227">
+        <v>1</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228">
+        <v>-0.4900000095367432</v>
+      </c>
+      <c r="B228">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C228">
+        <v>0.1000000238418579</v>
+      </c>
+      <c r="D228">
+        <v>1.256410360336304</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229">
+        <v>-1</v>
+      </c>
+      <c r="B229">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C229">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D229">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230">
+        <v>-1</v>
+      </c>
+      <c r="B230">
+        <v>1</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231">
+        <v>-1</v>
+      </c>
+      <c r="B231">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C231">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D231">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232">
+        <v>-1</v>
+      </c>
+      <c r="B232">
+        <v>1</v>
+      </c>
+      <c r="C232">
+        <v>0</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233">
+        <v>-1</v>
+      </c>
+      <c r="B233">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C233">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D233">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234">
+        <v>-1</v>
+      </c>
+      <c r="B234">
+        <v>1</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+      <c r="D234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235">
+        <v>-1</v>
+      </c>
+      <c r="B235">
+        <v>1</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236">
+        <v>-0.8399999737739563</v>
+      </c>
+      <c r="B236">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C236">
+        <v>0.449999988079071</v>
+      </c>
+      <c r="D236">
+        <v>2.153846263885498</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237">
+        <v>-1</v>
+      </c>
+      <c r="B237">
+        <v>0.3100000023841858</v>
+      </c>
+      <c r="C237">
+        <v>0.6899999976158142</v>
+      </c>
+      <c r="D237">
+        <v>3.225806474685669</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238">
+        <v>-2.039999961853027</v>
+      </c>
+      <c r="B238">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C238">
+        <v>1.649999976158142</v>
+      </c>
+      <c r="D238">
+        <v>5.230769157409668</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239">
+        <v>-1</v>
+      </c>
+      <c r="B239">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C239">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D239">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240">
+        <v>-1</v>
+      </c>
+      <c r="B240">
+        <v>1</v>
+      </c>
+      <c r="C240">
+        <v>0</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241">
+        <v>-1</v>
+      </c>
+      <c r="B241">
+        <v>1</v>
+      </c>
+      <c r="C241">
+        <v>0</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242">
+        <v>-1</v>
+      </c>
+      <c r="B242">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C242">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D242">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243">
+        <v>-0.5299999713897705</v>
+      </c>
+      <c r="B243">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C243">
+        <v>0.1399999856948853</v>
+      </c>
+      <c r="D243">
+        <v>1.35897433757782</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244">
+        <v>-1</v>
+      </c>
+      <c r="B244">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C244">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D244">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245">
+        <v>-1</v>
+      </c>
+      <c r="B245">
+        <v>0.3899999856948853</v>
+      </c>
+      <c r="C245">
+        <v>0.6100000143051147</v>
+      </c>
+      <c r="D245">
+        <v>2.564102649688721</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246">
+        <v>-0.3100000023841858</v>
+      </c>
+      <c r="B246">
+        <v>0.3100000023841858</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+      <c r="D246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247">
+        <v>-1</v>
+      </c>
+      <c r="B247">
+        <v>1</v>
+      </c>
+      <c r="C247">
+        <v>0</v>
+      </c>
+      <c r="D247">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>